<commit_message>
Modified code to support 2 level reading
</commit_message>
<xml_diff>
--- a/src/main/resources/input/students1.xlsx
+++ b/src/main/resources/input/students1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\suren\IdeaProjects\batch-excel\src\main\resources\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B48EC4F-6098-4CA6-99E5-2A59EFADBFD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA4CD571-F0F5-42B2-86AA-F51F674322D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1140" yWindow="1140" windowWidth="14400" windowHeight="7270" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>NAME</t>
   </si>
@@ -64,13 +64,40 @@
   </si>
   <si>
     <t>A1</t>
+  </si>
+  <si>
+    <t>John Smith 2</t>
+  </si>
+  <si>
+    <t>John Smith 3</t>
+  </si>
+  <si>
+    <t>John Smith 4</t>
+  </si>
+  <si>
+    <t>Male 2</t>
+  </si>
+  <si>
+    <t>Male 3</t>
+  </si>
+  <si>
+    <t>Male 4</t>
+  </si>
+  <si>
+    <t>A2</t>
+  </si>
+  <si>
+    <t>A3</t>
+  </si>
+  <si>
+    <t>A4</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -82,6 +109,12 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -406,10 +439,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -472,7 +505,50 @@
         <v>12</v>
       </c>
     </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6">
+        <v>19</v>
+      </c>
+      <c r="C6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7">
+        <v>20</v>
+      </c>
+      <c r="C7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8">
+        <v>21</v>
+      </c>
+      <c r="C8" t="s">
+        <v>18</v>
+      </c>
+      <c r="D8" t="s">
+        <v>21</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" xr:uid="{14F46A6D-06B8-4DBA-92F6-401AC3DB7957}"/>
     <hyperlink ref="B3" r:id="rId2" display="tony.tester@gmail.com" xr:uid="{E0BA4873-4296-48FC-BA21-FE30D54935D7}"/>

</xml_diff>